<commit_message>
add code for multiple testing cohorts
</commit_message>
<xml_diff>
--- a/LTS_ax_Problems_Tracker_rp.xlsx
+++ b/LTS_ax_Problems_Tracker_rp.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Patient</t>
   </si>
@@ -37,22 +37,10 @@
     <t>Fat_Mask_Size</t>
   </si>
   <si>
-    <t>Patient-035</t>
-  </si>
-  <si>
-    <t>Patient-056</t>
-  </si>
-  <si>
-    <t>Patient-075</t>
-  </si>
-  <si>
-    <t>Patient-080</t>
-  </si>
-  <si>
-    <t>Patient-088</t>
-  </si>
-  <si>
-    <t>Patient-089</t>
+    <t>Patient-093</t>
+  </si>
+  <si>
+    <t>Patient-094</t>
   </si>
 </sst>
 </file>
@@ -410,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -444,22 +432,22 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C2">
-        <v>485</v>
+        <v>990</v>
       </c>
       <c r="D2">
-        <v>203</v>
+        <v>317</v>
       </c>
       <c r="E2">
-        <v>450</v>
+        <v>639</v>
       </c>
       <c r="F2">
-        <v>637</v>
+        <v>858</v>
       </c>
       <c r="G2">
-        <v>1254</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -467,114 +455,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3">
-        <v>2073</v>
+        <v>430</v>
       </c>
       <c r="D3">
-        <v>188</v>
+        <v>15</v>
       </c>
       <c r="E3">
-        <v>425</v>
+        <v>122</v>
       </c>
       <c r="F3">
-        <v>591</v>
+        <v>283</v>
       </c>
       <c r="G3">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4">
-        <v>62</v>
-      </c>
-      <c r="C4">
-        <v>686</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
-        <v>121</v>
-      </c>
-      <c r="F4">
-        <v>237</v>
-      </c>
-      <c r="G4">
-        <v>1291</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5">
-        <v>38</v>
-      </c>
-      <c r="C5">
-        <v>404</v>
-      </c>
-      <c r="D5">
-        <v>68</v>
-      </c>
-      <c r="E5">
-        <v>98</v>
-      </c>
-      <c r="F5">
-        <v>113</v>
-      </c>
-      <c r="G5">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>48</v>
-      </c>
-      <c r="C6">
-        <v>1101</v>
-      </c>
-      <c r="D6">
-        <v>150</v>
-      </c>
-      <c r="E6">
-        <v>497</v>
-      </c>
-      <c r="F6">
-        <v>829</v>
-      </c>
-      <c r="G6">
-        <v>2682</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7">
-        <v>87</v>
-      </c>
-      <c r="C7">
-        <v>504</v>
-      </c>
-      <c r="D7">
-        <v>141</v>
-      </c>
-      <c r="E7">
-        <v>414</v>
-      </c>
-      <c r="F7">
-        <v>725</v>
-      </c>
-      <c r="G7">
-        <v>2402</v>
+        <v>779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>